<commit_message>
upgrade to v 1.0.16
</commit_message>
<xml_diff>
--- a/ExcelFile.net.Example.net40/C.xlsx
+++ b/ExcelFile.net.Example.net40/C.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="3470" windowWidth="14810" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="4030" windowWidth="14810" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>{s-Name}</t>
   </si>
@@ -27,6 +27,10 @@
   </si>
   <si>
     <t>Age</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Total</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -434,9 +438,14 @@
       <c r="E11" s="1"/>
     </row>
     <row r="12" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C12" s="1"/>
+      <c r="C12" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
+      <c r="E12" s="1">
+        <f>SUM(E7:E11)</f>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>